<commit_message>
Script de validação no cadastro
</commit_message>
<xml_diff>
--- a/Documentação/BeeAware - Tabela de Backlogs.xlsx
+++ b/Documentação/BeeAware - Tabela de Backlogs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/samuel_barros_sptech_school/Documents/Documentos/Algoritmo/Aula 3/BeeAware/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{CFF07BFE-683F-415A-AF06-F6C792A63056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5518289-1748-491E-917B-EEDF8188156A}"/>
+  <xr:revisionPtr revIDLastSave="309" documentId="8_{CFF07BFE-683F-415A-AF06-F6C792A63056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5D32019-6123-468C-9B96-F98CE448E175}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10800" xr2:uid="{80543608-BEA4-49AF-8FFD-EA8F197C5E11}"/>
+    <workbookView minimized="1" xWindow="2490" yWindow="3015" windowWidth="14400" windowHeight="7785" xr2:uid="{80543608-BEA4-49AF-8FFD-EA8F197C5E11}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="135">
   <si>
     <t>Categoria</t>
   </si>
@@ -399,6 +399,48 @@
   </si>
   <si>
     <t>Configuração da VM para armazenar os dados capturados pelo sensor, e visualização pelo site.</t>
+  </si>
+  <si>
+    <t>RF 13</t>
+  </si>
+  <si>
+    <t>Um campo do site para entrar em contato caso ocorra alguma dúvida ou erro com o monitoramento.</t>
+  </si>
+  <si>
+    <t>Semana 5</t>
+  </si>
+  <si>
+    <t>Sprint 2.5</t>
+  </si>
+  <si>
+    <t>RF 14</t>
+  </si>
+  <si>
+    <t>Área para contato com o suporte</t>
+  </si>
+  <si>
+    <t>Tela de  login</t>
+  </si>
+  <si>
+    <t>O sistema deve ter uma tela para realizar o login de contas comuns e administradoras</t>
+  </si>
+  <si>
+    <t>pequeno</t>
+  </si>
+  <si>
+    <t>RF 14.1</t>
+  </si>
+  <si>
+    <t>Autenticação na tela de login</t>
+  </si>
+  <si>
+    <t>Ao realizar o login em uma conta comum ou administrativa deverá ser emitido um email para validar o login</t>
+  </si>
+  <si>
+    <t>médio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 2 </t>
   </si>
 </sst>
 </file>
@@ -512,17 +554,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -533,11 +564,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -578,14 +618,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -907,8 +962,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FED80B8D-399D-4E7A-9809-08A663DD6FC0}" name="Tabela1" displayName="Tabela1" ref="A1:J32" insertRowShift="1" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J32" xr:uid="{FED80B8D-399D-4E7A-9809-08A663DD6FC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FED80B8D-399D-4E7A-9809-08A663DD6FC0}" name="Tabela1" displayName="Tabela1" ref="A1:J35" insertRowShift="1" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J35" xr:uid="{FED80B8D-399D-4E7A-9809-08A663DD6FC0}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{D4DB35A4-7BDA-47B8-9146-DC991559B1AB}" name="Categoria" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{7CE056E5-82A8-4ED5-9A11-1948EC8B7BAD}" name="Identificador" dataDxfId="8"/>
@@ -1242,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C758E312-D0F0-47C3-BE6E-1CB40388AC50}">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="88" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1317,7 @@
     <col min="10" max="10" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1293,12 +1348,8 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="M1" s="16"/>
-    </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1329,15 +1380,8 @@
       <c r="J2" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="M2" s="11">
-        <f>SUM(H:H)</f>
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1368,15 +1412,8 @@
       <c r="J3" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="L3" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" s="13">
-        <f>SUM(H2,H4,H5,H12,H14,H16,H21,H23,H25,H26,H27,H28,H31,)</f>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1407,15 +1444,8 @@
       <c r="J4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="L4" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="M4" s="13">
-        <f>SUM(H22,H24,H29,H30,H32,)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1446,15 +1476,8 @@
       <c r="J5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="L5" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="M5" s="13">
-        <f>SUM(H3,H13,H15,H19,H20,)</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1485,15 +1508,8 @@
       <c r="J6" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="L6" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="M6" s="13">
-        <f>SUM(H17,H18,)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1524,15 +1540,8 @@
       <c r="J7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="L7" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="M7" s="15">
-        <f>SUM(H6,H7,H8,Tabela1[[#This Row],[Tam('#)]],H10,H11,)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1564,7 +1573,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1596,7 +1605,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1660,7 +1669,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1692,7 +1701,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -1724,7 +1733,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1756,7 +1765,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -2141,157 +2150,157 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="9">
+      <c r="A27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="17">
+        <v>3</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H27" s="18">
+        <v>3</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="17">
         <v>1</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H27" s="9">
+      <c r="G28" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H28" s="18">
         <v>5</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="9">
-        <v>3</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H28" s="9">
-        <v>5</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>98</v>
+      <c r="I28" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="A29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="9">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H29" s="9">
-        <v>13</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="F29" s="17">
+        <v>2</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="H29" s="18">
+        <v>8</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F30" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H30" s="9">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="F31" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H31" s="9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I31" s="9" t="s">
         <v>96</v>
@@ -2300,30 +2309,30 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F32" s="9">
         <v>1</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H32" s="9">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="I32" s="9" t="s">
         <v>97</v>
@@ -2332,41 +2341,101 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="9">
+        <v>3</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H33" s="9">
+        <v>13</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="9">
+        <v>8</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35" s="9">
+        <v>8</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
@@ -2374,15 +2443,17 @@
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
+      <c r="A37" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="14"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="3"/>
@@ -2393,8 +2464,13 @@
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
+      <c r="A38" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="11">
+        <f>SUM(H:H)</f>
+        <v>215</v>
+      </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="3"/>
@@ -2405,8 +2481,13 @@
       <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
+      <c r="A39" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="13">
+        <f>SUM(H2,H4,H5,H12,H14,H16,H21,H23,H25,H26,H30,H31,H34,)</f>
+        <v>84</v>
+      </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="3"/>
@@ -2417,8 +2498,13 @@
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
+      <c r="A40" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="13">
+        <f>SUM(H22,H24,H32,H33,H35,)</f>
+        <v>40</v>
+      </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="3"/>
@@ -2429,8 +2515,13 @@
       <c r="J40" s="7"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
+      <c r="A41" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" s="13">
+        <f>SUM(H3,H13,H15,H19,H20,)</f>
+        <v>29</v>
+      </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="3"/>
@@ -2441,8 +2532,13 @@
       <c r="J41" s="7"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
+      <c r="A42" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" s="13">
+        <f>SUM(H17,H18,)</f>
+        <v>16</v>
+      </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="3"/>
@@ -2453,8 +2549,13 @@
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
+      <c r="A43" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="13">
+        <f>SUM(H11,H10,H9,H8,H7,H6,)</f>
+        <v>30</v>
+      </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="3"/>
@@ -2465,8 +2566,13 @@
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
+      <c r="A44" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="21">
+        <f>SUM(H27:H29)</f>
+        <v>16</v>
+      </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="3"/>
@@ -2488,9 +2594,45 @@
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
     </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A37:B37"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Adição da tabela das sprints semanais
</commit_message>
<xml_diff>
--- a/Documentação/BeeAware - Tabela de Backlogs.xlsx
+++ b/Documentação/BeeAware - Tabela de Backlogs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/samuel_barros_sptech_school/Documents/Documentos/Algoritmo/Aula 3/BeeAware/Documentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/samuel_barros_sptech_school/Documents/Área de Trabalho/BeeAware/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="309" documentId="8_{CFF07BFE-683F-415A-AF06-F6C792A63056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5D32019-6123-468C-9B96-F98CE448E175}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="8_{CFF07BFE-683F-415A-AF06-F6C792A63056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C10FF7A3-BF52-430A-919B-4F53349E1505}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2490" yWindow="3015" windowWidth="14400" windowHeight="7785" xr2:uid="{80543608-BEA4-49AF-8FFD-EA8F197C5E11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{80543608-BEA4-49AF-8FFD-EA8F197C5E11}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="122">
   <si>
     <t>Categoria</t>
   </si>
@@ -401,46 +401,7 @@
     <t>Configuração da VM para armazenar os dados capturados pelo sensor, e visualização pelo site.</t>
   </si>
   <si>
-    <t>RF 13</t>
-  </si>
-  <si>
-    <t>Um campo do site para entrar em contato caso ocorra alguma dúvida ou erro com o monitoramento.</t>
-  </si>
-  <si>
-    <t>Semana 5</t>
-  </si>
-  <si>
     <t>Sprint 2.5</t>
-  </si>
-  <si>
-    <t>RF 14</t>
-  </si>
-  <si>
-    <t>Área para contato com o suporte</t>
-  </si>
-  <si>
-    <t>Tela de  login</t>
-  </si>
-  <si>
-    <t>O sistema deve ter uma tela para realizar o login de contas comuns e administradoras</t>
-  </si>
-  <si>
-    <t>pequeno</t>
-  </si>
-  <si>
-    <t>RF 14.1</t>
-  </si>
-  <si>
-    <t>Autenticação na tela de login</t>
-  </si>
-  <si>
-    <t>Ao realizar o login em uma conta comum ou administrativa deverá ser emitido um email para validar o login</t>
-  </si>
-  <si>
-    <t>médio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 2 </t>
   </si>
 </sst>
 </file>
@@ -619,6 +580,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -632,15 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -962,8 +923,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FED80B8D-399D-4E7A-9809-08A663DD6FC0}" name="Tabela1" displayName="Tabela1" ref="A1:J35" insertRowShift="1" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J35" xr:uid="{FED80B8D-399D-4E7A-9809-08A663DD6FC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FED80B8D-399D-4E7A-9809-08A663DD6FC0}" name="Tabela1" displayName="Tabela1" ref="A1:J32" insertRowShift="1" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J32" xr:uid="{FED80B8D-399D-4E7A-9809-08A663DD6FC0}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{D4DB35A4-7BDA-47B8-9146-DC991559B1AB}" name="Categoria" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{7CE056E5-82A8-4ED5-9A11-1948EC8B7BAD}" name="Identificador" dataDxfId="8"/>
@@ -1299,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C758E312-D0F0-47C3-BE6E-1CB40388AC50}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="88" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2131,7 +2092,7 @@
         <v>118</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F26" s="9">
         <v>1</v>
@@ -2150,292 +2111,232 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="E27" s="15" t="s">
+      <c r="A27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" s="9">
+        <v>5</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="9">
+        <v>3</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" s="9">
+        <v>5</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F29" s="9">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" s="9">
+        <v>13</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="20">
         <v>3</v>
       </c>
-      <c r="G27" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="H27" s="18">
-        <v>3</v>
-      </c>
-      <c r="I27" s="18" t="s">
+      <c r="G30" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="21">
+        <v>13</v>
+      </c>
+      <c r="I30" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="J27" s="18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="17">
+      <c r="J30" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="20">
         <v>1</v>
       </c>
-      <c r="G28" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="H28" s="18">
-        <v>5</v>
-      </c>
-      <c r="I28" s="18" t="s">
+      <c r="G31" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" s="21">
+        <v>8</v>
+      </c>
+      <c r="I31" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="20">
+        <v>1</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H32" s="21">
+        <v>8</v>
+      </c>
+      <c r="I32" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="J28" s="18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="17">
-        <v>2</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="H29" s="18">
-        <v>8</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="9">
-        <v>1</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H30" s="9">
-        <v>5</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="9">
-        <v>3</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H31" s="9">
-        <v>5</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="9">
-        <v>1</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H32" s="9">
-        <v>13</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="J32" s="9" t="s">
+      <c r="J32" s="21" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="9">
-        <v>3</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H33" s="9">
-        <v>13</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="9">
-        <v>1</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H34" s="9">
-        <v>8</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="9">
-        <v>1</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H35" s="9">
-        <v>8</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>102</v>
-      </c>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
@@ -2450,10 +2351,10 @@
       <c r="J36" s="9"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="14"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="3"/>
@@ -2469,7 +2370,7 @@
       </c>
       <c r="B38" s="11">
         <f>SUM(H:H)</f>
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -2485,7 +2386,7 @@
         <v>96</v>
       </c>
       <c r="B39" s="13">
-        <f>SUM(H2,H4,H5,H12,H14,H16,H21,H23,H25,H26,H30,H31,H34,)</f>
+        <f>SUM(H2,H4,H5,H12,H14,H16,H21,H23,H25,H26,H27,H28,H31,)</f>
         <v>84</v>
       </c>
       <c r="C39" s="4"/>
@@ -2502,7 +2403,7 @@
         <v>107</v>
       </c>
       <c r="B40" s="13">
-        <f>SUM(H22,H24,H32,H33,H35,)</f>
+        <f>SUM(H22,H24,H29,H30,H32,)</f>
         <v>40</v>
       </c>
       <c r="C40" s="4"/>
@@ -2549,7 +2450,7 @@
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="14" t="s">
         <v>106</v>
       </c>
       <c r="B43" s="13">
@@ -2566,12 +2467,12 @@
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B44" s="21">
-        <f>SUM(H27:H29)</f>
-        <v>16</v>
+      <c r="A44" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="16" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>

</xml_diff>